<commit_message>
Update reflection comparision 3_23_22.xlsx
</commit_message>
<xml_diff>
--- a/Reflection/reflection comparision 3_23_22.xlsx
+++ b/Reflection/reflection comparision 3_23_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9775220ff73936ab/Documents/GitHub/AutoCIF/Reflection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B70DA597-41A3-49F5-B12A-51774CC162B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{B70DA597-41A3-49F5-B12A-51774CC162B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13CB10BA-75B2-4B95-942F-196573C6D619}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A702E7F-2E91-4729-A239-963DB022218A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>sample</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>maxi black is 25x better than black spray paint</t>
+  </si>
+  <si>
+    <t>maxi black is about 35,000x better than uncoated blue PLA</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FE6933-EF76-4AC9-A388-D9532529491E}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,6 +498,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>